<commit_message>
changes hourly increments into 15-min quarters, from 30-minutes. also adds time scale to right side of the table as well. moves legend up to top of screen in anticipation for more categories
</commit_message>
<xml_diff>
--- a/Template-Weekly-Productivity-Log.xlsx
+++ b/Template-Weekly-Productivity-Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/867acb827b40e744/Desktop/Projects/Sheetz/Sheetz/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/867acb827b40e744/Desktop/PROJECTS/Sheetz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22DE2862-562D-4ED2-8F0B-DB4397831CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{22DE2862-562D-4ED2-8F0B-DB4397831CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4528F2D5-36BD-4B6E-9771-B674BA0A3DC1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85B57D0C-48D7-40D2-9C68-89B4036B9F4C}"/>
   </bookViews>
@@ -715,9 +715,6 @@
   </cellStyleXfs>
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -742,9 +739,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,15 +836,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -874,12 +859,105 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7AA5CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66CC77"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9966CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF999999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FF66CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD8BFD8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB0E57C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA2B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -993,13 +1071,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color rgb="FF000000"/>
@@ -1011,6 +1082,13 @@
           <color rgb="FF000000"/>
         </top>
         <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
@@ -1031,84 +1109,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7AA5CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66CC77"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9966CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FF66CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD8BFD8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB0E57C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFA2B6"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1123,16 +1123,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EEECB1C-857F-4B02-8AAF-C4CD15CB68CB}" name="Table47234" displayName="Table47234" ref="J1:M12" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EEECB1C-857F-4B02-8AAF-C4CD15CB68CB}" name="Table47234" displayName="Table47234" ref="J1:M12" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="J1:M12" xr:uid="{22E8C784-274F-494D-8AE3-75E551D2A9DA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J2:L10">
     <sortCondition ref="J1:J10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{70349FDD-3CA2-4FC7-8A16-1CF3D5A8C5F5}" name="ITEM" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{E559AD58-2035-4859-9A40-F69860E54668}" name="DESCRIPTION" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B756A8C9-3EC2-4BB6-A1F1-E5C532A6837C}" name="COLOR" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{6FFFA0A4-C25E-4F02-A7F4-B52AD8E8D20F}" name="HEX" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{70349FDD-3CA2-4FC7-8A16-1CF3D5A8C5F5}" name="ITEM" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{E559AD58-2035-4859-9A40-F69860E54668}" name="DESCRIPTION" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B756A8C9-3EC2-4BB6-A1F1-E5C532A6837C}" name="COLOR" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{6FFFA0A4-C25E-4F02-A7F4-B52AD8E8D20F}" name="HEX" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1441,12 +1441,12 @@
   <dimension ref="A1:M117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="54" customWidth="1"/>
+    <col min="1" max="1" width="11" style="49" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -1455,1638 +1455,1638 @@
     <col min="13" max="13" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="50"/>
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="1:13" s="8" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="51"/>
+      <c r="J2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="16">
         <v>0</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="18">
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="16">
         <v>0</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="22" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="23">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="26">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="28">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="26">
         <v>2.0833333333333301E-2</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="21">
         <v>3.125E-2</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="23">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="21">
         <v>3.125E-2</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="26">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="28">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="26">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="34" t="s">
+      <c r="L7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="21">
         <v>5.2083333333333301E-2</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="23">
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="21">
         <v>5.2083333333333301E-2</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="35" t="s">
+      <c r="K8" s="13"/>
+      <c r="L8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="15">
         <v>999999</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="26">
         <v>6.25E-2</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="28">
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="26">
         <v>6.25E-2</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="21">
         <v>7.2916666666666699E-2</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="23">
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="21">
         <v>7.2916666666666699E-2</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="26">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="28">
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="26">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="21">
         <v>9.375E-2</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="23">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="21">
         <v>9.375E-2</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="39" t="s">
+      <c r="L12" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="26">
         <v>0.104166666666667</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="28">
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="26">
         <v>0.104166666666667</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
+      <c r="A14" s="21">
         <v>0.114583333333333</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="23">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="21">
         <v>0.114583333333333</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="26">
         <v>0.125</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="28">
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="26">
         <v>0.125</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="21">
         <v>0.13541666666666699</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="23">
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="21">
         <v>0.13541666666666699</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="26">
         <v>0.14583333333333301</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="28">
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="26">
         <v>0.14583333333333301</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
+      <c r="A18" s="21">
         <v>0.15625</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="23">
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="21">
         <v>0.15625</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28">
+      <c r="A19" s="26">
         <v>0.16666666666666699</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="28">
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="26">
         <v>0.16666666666666699</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+      <c r="A20" s="21">
         <v>0.17708333333333301</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="23">
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="21">
         <v>0.17708333333333301</v>
       </c>
-      <c r="K20" s="40"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="26">
         <v>0.1875</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="28">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="26">
         <v>0.1875</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
+      <c r="A22" s="21">
         <v>0.19791666666666699</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="23">
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="21">
         <v>0.19791666666666699</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28">
+      <c r="A23" s="26">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="28">
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="26">
         <v>0.20833333333333301</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
+      <c r="A24" s="21">
         <v>0.21875</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="23">
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="21">
         <v>0.21875</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="A25" s="26">
         <v>0.22916666666666699</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="28">
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="26">
         <v>0.22916666666666699</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
+      <c r="A26" s="21">
         <v>0.23958333333333301</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="23">
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="21">
         <v>0.23958333333333301</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28">
+      <c r="A27" s="26">
         <v>0.25</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="28">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="26">
         <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="21">
         <v>0.26041666666666702</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="23">
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="21">
         <v>0.26041666666666702</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28">
+      <c r="A29" s="26">
         <v>0.27083333333333298</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="28">
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="26">
         <v>0.27083333333333298</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
+      <c r="A30" s="21">
         <v>0.28125</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="23">
+      <c r="B30" s="22"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="21">
         <v>0.28125</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28">
+      <c r="A31" s="26">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="28">
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="26">
         <v>0.29166666666666702</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
+      <c r="A32" s="21">
         <v>0.30208333333333298</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="23">
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="21">
         <v>0.30208333333333298</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28">
+      <c r="A33" s="26">
         <v>0.3125</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="28">
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="26">
         <v>0.3125</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23">
+      <c r="A34" s="21">
         <v>0.32291666666666702</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="23">
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="21">
         <v>0.32291666666666702</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28">
+      <c r="A35" s="26">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="28">
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="26">
         <v>0.33333333333333298</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23">
+      <c r="A36" s="21">
         <v>0.343749999999999</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="23">
+      <c r="B36" s="22"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="21">
         <v>0.343749999999999</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+      <c r="A37" s="26">
         <v>0.35416666666666502</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="28">
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="26">
         <v>0.35416666666666502</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23">
+      <c r="A38" s="21">
         <v>0.36458333333333098</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="23">
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="21">
         <v>0.36458333333333098</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="A39" s="26">
         <v>0.374999999999997</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="28">
+      <c r="B39" s="27"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="26">
         <v>0.374999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23">
+      <c r="A40" s="21">
         <v>0.38541666666666302</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="23">
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="21">
         <v>0.38541666666666302</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28">
+      <c r="A41" s="26">
         <v>0.39583333333332898</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="28">
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="26">
         <v>0.39583333333332898</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23">
+      <c r="A42" s="21">
         <v>0.406249999999995</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="23">
+      <c r="B42" s="22"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="21">
         <v>0.406249999999995</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28">
+      <c r="A43" s="26">
         <v>0.41666666666666102</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="28">
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="26">
         <v>0.41666666666666102</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23">
+      <c r="A44" s="21">
         <v>0.42708333333332699</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="23">
+      <c r="B44" s="22"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="21">
         <v>0.42708333333332699</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28">
+      <c r="A45" s="26">
         <v>0.43749999999999301</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="28">
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="26">
         <v>0.43749999999999301</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="23">
+      <c r="A46" s="21">
         <v>0.44791666666665902</v>
       </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="23">
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="21">
         <v>0.44791666666665902</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="28">
+      <c r="A47" s="26">
         <v>0.45833333333332499</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="28">
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="26">
         <v>0.45833333333332499</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="23">
+      <c r="A48" s="21">
         <v>0.46874999999999101</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="23">
+      <c r="B48" s="22"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="21">
         <v>0.46874999999999101</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="28">
+      <c r="A49" s="26">
         <v>0.47916666666665703</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="28">
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="26">
         <v>0.47916666666665703</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="23">
+      <c r="A50" s="21">
         <v>0.48958333333332299</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="23">
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="21">
         <v>0.48958333333332299</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="28">
+      <c r="A51" s="26">
         <v>0.49999999999998901</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="28">
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="26">
         <v>0.49999999999998901</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
+      <c r="A52" s="21">
         <v>0.51041666666665497</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="23">
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="21">
         <v>0.51041666666665497</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="28">
+      <c r="A53" s="26">
         <v>0.52083333333332105</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="28">
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="26">
         <v>0.52083333333332105</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="23">
+      <c r="A54" s="21">
         <v>0.53124999999998701</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="23">
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="21">
         <v>0.53124999999998701</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="28">
+      <c r="A55" s="26">
         <v>0.54166666666665297</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="28">
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="26">
         <v>0.54166666666665297</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="23">
+      <c r="A56" s="21">
         <v>0.55208333333331905</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="23">
+      <c r="B56" s="22"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="21">
         <v>0.55208333333331905</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="28">
+      <c r="A57" s="26">
         <v>0.56249999999998501</v>
       </c>
-      <c r="B57" s="29"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="28">
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="26">
         <v>0.56249999999998501</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="23">
+      <c r="A58" s="21">
         <v>0.57291666666665098</v>
       </c>
-      <c r="B58" s="24"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="23">
+      <c r="B58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="21">
         <v>0.57291666666665098</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="28">
+      <c r="A59" s="26">
         <v>0.58333333333331705</v>
       </c>
-      <c r="B59" s="29"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="28">
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="26">
         <v>0.58333333333331705</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="23">
+      <c r="A60" s="21">
         <v>0.59374999999998201</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="23">
+      <c r="B60" s="22"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="21">
         <v>0.59374999999998201</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="28">
+      <c r="A61" s="26">
         <v>0.60416666666664798</v>
       </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="28">
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="26">
         <v>0.60416666666664798</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="23">
+      <c r="A62" s="21">
         <v>0.61458333333331405</v>
       </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="23">
+      <c r="B62" s="22"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="21">
         <v>0.61458333333331405</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="28">
+      <c r="A63" s="26">
         <v>0.62499999999998002</v>
       </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="28">
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="26">
         <v>0.62499999999998002</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="23">
+      <c r="A64" s="21">
         <v>0.63541666666664598</v>
       </c>
-      <c r="B64" s="24"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="26"/>
-      <c r="I64" s="23">
+      <c r="B64" s="22"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="21">
         <v>0.63541666666664598</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="28">
+      <c r="A65" s="26">
         <v>0.64583333333331205</v>
       </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="28">
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="26">
         <v>0.64583333333331205</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="23">
+      <c r="A66" s="21">
         <v>0.65624999999997802</v>
       </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="23">
+      <c r="B66" s="22"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="21">
         <v>0.65624999999997802</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="28">
+      <c r="A67" s="26">
         <v>0.66666666666664398</v>
       </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="31"/>
-      <c r="I67" s="28">
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="26">
         <v>0.66666666666664398</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
+      <c r="A68" s="21">
         <v>0.67708333333330994</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="26"/>
-      <c r="I68" s="23">
+      <c r="B68" s="22"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="21">
         <v>0.67708333333330994</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="28">
+      <c r="A69" s="26">
         <v>0.68749999999997602</v>
       </c>
-      <c r="B69" s="29"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="31"/>
-      <c r="I69" s="28">
+      <c r="B69" s="27"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="26">
         <v>0.68749999999997602</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
+      <c r="A70" s="21">
         <v>0.69791666666664198</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="23">
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="23"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="21">
         <v>0.69791666666664198</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="28">
+      <c r="A71" s="26">
         <v>0.70833333333330795</v>
       </c>
-      <c r="B71" s="29"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="28">
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="26">
         <v>0.70833333333330795</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="23">
+      <c r="A72" s="21">
         <v>0.71874999999997402</v>
       </c>
-      <c r="B72" s="24"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-      <c r="H72" s="26"/>
-      <c r="I72" s="23">
+      <c r="B72" s="22"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="21">
         <v>0.71874999999997402</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="28">
+      <c r="A73" s="26">
         <v>0.72916666666663998</v>
       </c>
-      <c r="B73" s="29"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="28">
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="26">
         <v>0.72916666666663998</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="23">
+      <c r="A74" s="21">
         <v>0.73958333333330595</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="26"/>
-      <c r="I74" s="23">
+      <c r="B74" s="22"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="21">
         <v>0.73958333333330595</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="28">
+      <c r="A75" s="26">
         <v>0.74999999999997202</v>
       </c>
-      <c r="B75" s="29"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="31"/>
-      <c r="I75" s="28">
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="26">
         <v>0.74999999999997202</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="23">
+      <c r="A76" s="21">
         <v>0.76041666666663799</v>
       </c>
-      <c r="B76" s="24"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="26"/>
-      <c r="I76" s="23">
+      <c r="B76" s="22"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="21">
         <v>0.76041666666663799</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="28">
+      <c r="A77" s="26">
         <v>0.77083333333330395</v>
       </c>
-      <c r="B77" s="29"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
-      <c r="G77" s="30"/>
-      <c r="H77" s="31"/>
-      <c r="I77" s="28">
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="26">
         <v>0.77083333333330395</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="23">
+      <c r="A78" s="21">
         <v>0.78124999999997002</v>
       </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-      <c r="H78" s="26"/>
-      <c r="I78" s="23">
+      <c r="B78" s="22"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="21">
         <v>0.78124999999997002</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="28">
+      <c r="A79" s="26">
         <v>0.79166666666663699</v>
       </c>
-      <c r="B79" s="29"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
-      <c r="G79" s="30"/>
-      <c r="H79" s="31"/>
-      <c r="I79" s="28">
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="26">
         <v>0.79166666666663699</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="23">
+      <c r="A80" s="21">
         <v>0.80208333333330295</v>
       </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="26"/>
-      <c r="I80" s="23">
+      <c r="B80" s="22"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="21">
         <v>0.80208333333330295</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="28">
+      <c r="A81" s="26">
         <v>0.81249999999996902</v>
       </c>
-      <c r="B81" s="29"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
-      <c r="E81" s="30"/>
-      <c r="F81" s="30"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="31"/>
-      <c r="I81" s="28">
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="26">
         <v>0.81249999999996902</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="23">
+      <c r="A82" s="21">
         <v>0.82291666666663499</v>
       </c>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="25"/>
-      <c r="H82" s="26"/>
-      <c r="I82" s="23">
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="21">
         <v>0.82291666666663499</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="28">
+      <c r="A83" s="26">
         <v>0.83333333333330095</v>
       </c>
-      <c r="B83" s="29"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
-      <c r="E83" s="30"/>
-      <c r="F83" s="30"/>
-      <c r="G83" s="30"/>
-      <c r="H83" s="31"/>
-      <c r="I83" s="28">
+      <c r="B83" s="27"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="26">
         <v>0.83333333333330095</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="23">
+      <c r="A84" s="21">
         <v>0.84374999999996703</v>
       </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="25"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="23">
+      <c r="B84" s="22"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="21">
         <v>0.84374999999996703</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="28">
+      <c r="A85" s="26">
         <v>0.85416666666663299</v>
       </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="30"/>
-      <c r="G85" s="30"/>
-      <c r="H85" s="31"/>
-      <c r="I85" s="28">
+      <c r="B85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="28"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="26">
         <v>0.85416666666663299</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="23">
+      <c r="A86" s="21">
         <v>0.86458333333329895</v>
       </c>
-      <c r="B86" s="41"/>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="42"/>
-      <c r="F86" s="42"/>
-      <c r="G86" s="42"/>
-      <c r="H86" s="43"/>
-      <c r="I86" s="23">
+      <c r="B86" s="39"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="40"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="40"/>
+      <c r="H86" s="41"/>
+      <c r="I86" s="21">
         <v>0.86458333333329895</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="28">
+      <c r="A87" s="26">
         <v>0.87499999999996303</v>
       </c>
-      <c r="B87" s="44" t="s">
+      <c r="B87" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="45"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="45"/>
-      <c r="H87" s="46"/>
-      <c r="I87" s="28">
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="53"/>
+      <c r="G87" s="53"/>
+      <c r="H87" s="54"/>
+      <c r="I87" s="26">
         <v>0.87499999999996303</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="23">
+      <c r="A88" s="21">
         <v>0.88541666666662899</v>
       </c>
-      <c r="B88" s="47"/>
-      <c r="C88" s="48"/>
-      <c r="D88" s="48"/>
-      <c r="E88" s="48"/>
-      <c r="F88" s="48"/>
-      <c r="G88" s="48"/>
-      <c r="H88" s="49"/>
-      <c r="I88" s="23">
+      <c r="B88" s="42"/>
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="43"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="21">
         <v>0.88541666666662899</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="28">
+      <c r="A89" s="26">
         <v>0.89583333333329496</v>
       </c>
-      <c r="B89" s="29"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="30"/>
-      <c r="G89" s="30"/>
-      <c r="H89" s="31"/>
-      <c r="I89" s="28">
+      <c r="B89" s="27"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="26">
         <v>0.89583333333329496</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="23">
+      <c r="A90" s="21">
         <v>0.90624999999996103</v>
       </c>
-      <c r="B90" s="24"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="26"/>
-      <c r="I90" s="23">
+      <c r="B90" s="22"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="21">
         <v>0.90624999999996103</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="28">
+      <c r="A91" s="26">
         <v>0.91666666666662699</v>
       </c>
-      <c r="B91" s="29"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="30"/>
-      <c r="G91" s="30"/>
-      <c r="H91" s="31"/>
-      <c r="I91" s="28">
+      <c r="B91" s="27"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="28"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="26">
         <v>0.91666666666662699</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="23">
+      <c r="A92" s="21">
         <v>0.92708333333329296</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="25"/>
-      <c r="H92" s="26"/>
-      <c r="I92" s="23">
+      <c r="B92" s="22"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="21">
         <v>0.92708333333329296</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="28">
+      <c r="A93" s="26">
         <v>0.93749999999995903</v>
       </c>
-      <c r="B93" s="29"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="30"/>
-      <c r="G93" s="30"/>
-      <c r="H93" s="31"/>
-      <c r="I93" s="28">
+      <c r="B93" s="27"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="28"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="26">
         <v>0.93749999999995903</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="23">
+      <c r="A94" s="21">
         <v>0.947916666666625</v>
       </c>
-      <c r="B94" s="24"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="25"/>
-      <c r="H94" s="26"/>
-      <c r="I94" s="23">
+      <c r="B94" s="22"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="21">
         <v>0.947916666666625</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="28">
+      <c r="A95" s="26">
         <v>0.95833333333329096</v>
       </c>
-      <c r="B95" s="29"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="30"/>
-      <c r="G95" s="30"/>
-      <c r="H95" s="31"/>
-      <c r="I95" s="28">
+      <c r="B95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="28"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="26">
         <v>0.95833333333329096</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="23">
+      <c r="A96" s="21">
         <v>0.96874999999995703</v>
       </c>
-      <c r="B96" s="24"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="25"/>
-      <c r="H96" s="26"/>
-      <c r="I96" s="23">
+      <c r="B96" s="22"/>
+      <c r="C96" s="23"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="21">
         <v>0.96874999999995703</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="28">
+      <c r="A97" s="26">
         <v>0.979166666666623</v>
       </c>
-      <c r="B97" s="29"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
-      <c r="G97" s="30"/>
-      <c r="H97" s="31"/>
-      <c r="I97" s="28">
+      <c r="B97" s="27"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="26">
         <v>0.979166666666623</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="50">
+      <c r="A98" s="45">
         <v>0.98958333333328896</v>
       </c>
-      <c r="B98" s="51"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
-      <c r="E98" s="52"/>
-      <c r="F98" s="52"/>
-      <c r="G98" s="52"/>
-      <c r="H98" s="53"/>
-      <c r="I98" s="50">
+      <c r="B98" s="46"/>
+      <c r="C98" s="47"/>
+      <c r="D98" s="47"/>
+      <c r="E98" s="47"/>
+      <c r="F98" s="47"/>
+      <c r="G98" s="47"/>
+      <c r="H98" s="48"/>
+      <c r="I98" s="45">
         <v>0.98958333333328896</v>
       </c>
     </row>
@@ -3104,37 +3104,37 @@
     <mergeCell ref="B87:H87"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:H22 B24:H86 B88:H98">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>B3=$J$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>B3=$J$11</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>B3=$J$10</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>B3=$J$9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>B3=$J$8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>B3=$J$7</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>B3=$J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>B3=$J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>B3=$J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>B3=$J$3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="0" priority="11">
       <formula>B3=$J$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
.gitignore should work now and stops tracking ignored files.. that was a learning experiance. always rm --cached ignore -r after files that were previously tracked are added to .gitignore
</commit_message>
<xml_diff>
--- a/Template-Weekly-Productivity-Log.xlsx
+++ b/Template-Weekly-Productivity-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/867acb827b40e744/Desktop/PROJECTS/Sheetz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{22DE2862-562D-4ED2-8F0B-DB4397831CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9577DA54-2E6D-46AB-A562-6CF5DAD8844A}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{22DE2862-562D-4ED2-8F0B-DB4397831CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88CBEB16-6B01-42F9-A7E1-C1A88DFC0F89}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85B57D0C-48D7-40D2-9C68-89B4036B9F4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>MON</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>SCHEDULED BEDTIME</t>
-  </si>
-  <si>
-    <t>HI ALYSSIA!!!</t>
   </si>
 </sst>
 </file>
@@ -344,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -533,21 +530,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -739,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -828,29 +810,34 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,16 +846,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,7 +861,7 @@
     <xf numFmtId="20" fontId="1" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -892,13 +873,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1471,12 +1452,12 @@
   <dimension ref="A1:M117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -1486,7 +1467,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
+      <c r="A1" s="49"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1486,7 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="36" t="s">
         <v>6</v>
       </c>
       <c r="I1"/>
@@ -1523,7 +1504,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1542,7 +1523,7 @@
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="37" t="s">
         <v>11</v>
       </c>
       <c r="I2"/>
@@ -1560,7 +1541,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
+      <c r="A3" s="44">
         <v>0</v>
       </c>
       <c r="B3" s="14"/>
@@ -1569,7 +1550,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="39"/>
+      <c r="H3" s="38"/>
       <c r="J3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1582,7 +1563,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46">
+      <c r="A4" s="45">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="B4" s="17"/>
@@ -1591,7 +1572,7 @@
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="40"/>
+      <c r="H4" s="39"/>
       <c r="J4" s="10" t="s">
         <v>19</v>
       </c>
@@ -1606,7 +1587,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47">
+      <c r="A5" s="46">
         <v>2.0833333333333301E-2</v>
       </c>
       <c r="B5" s="20"/>
@@ -1615,7 +1596,7 @@
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="41"/>
+      <c r="H5" s="40"/>
       <c r="J5" s="10" t="s">
         <v>23</v>
       </c>
@@ -1630,7 +1611,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46">
+      <c r="A6" s="45">
         <v>3.125E-2</v>
       </c>
       <c r="B6" s="17"/>
@@ -1639,7 +1620,7 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="40"/>
+      <c r="H6" s="39"/>
       <c r="J6" s="10" t="s">
         <v>27</v>
       </c>
@@ -1654,7 +1635,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="A7" s="46">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="B7" s="20"/>
@@ -1663,7 +1644,7 @@
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="41"/>
+      <c r="H7" s="40"/>
       <c r="J7" s="10" t="s">
         <v>31</v>
       </c>
@@ -1678,7 +1659,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46">
+      <c r="A8" s="45">
         <v>5.2083333333333301E-2</v>
       </c>
       <c r="B8" s="17"/>
@@ -1687,7 +1668,7 @@
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
-      <c r="H8" s="40"/>
+      <c r="H8" s="39"/>
       <c r="J8" s="10" t="s">
         <v>35</v>
       </c>
@@ -1700,7 +1681,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="46">
         <v>6.25E-2</v>
       </c>
       <c r="B9" s="20"/>
@@ -1709,7 +1690,7 @@
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="41"/>
+      <c r="H9" s="40"/>
       <c r="J9" s="10" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1705,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46">
+      <c r="A10" s="45">
         <v>7.2916666666666699E-2</v>
       </c>
       <c r="B10" s="17"/>
@@ -1733,7 +1714,7 @@
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
-      <c r="H10" s="40"/>
+      <c r="H10" s="39"/>
       <c r="J10" s="10" t="s">
         <v>41</v>
       </c>
@@ -1748,7 +1729,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47">
+      <c r="A11" s="46">
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B11" s="20"/>
@@ -1757,7 +1738,7 @@
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="41"/>
+      <c r="H11" s="40"/>
       <c r="J11" s="10" t="s">
         <v>45</v>
       </c>
@@ -1772,7 +1753,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46">
+      <c r="A12" s="45">
         <v>9.375E-2</v>
       </c>
       <c r="B12" s="17"/>
@@ -1781,7 +1762,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
-      <c r="H12" s="40"/>
+      <c r="H12" s="39"/>
       <c r="J12" s="10" t="s">
         <v>49</v>
       </c>
@@ -1796,7 +1777,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
+      <c r="A13" s="46">
         <v>0.104166666666667</v>
       </c>
       <c r="B13" s="20"/>
@@ -1805,10 +1786,10 @@
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="41"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="45">
         <v>0.114583333333333</v>
       </c>
       <c r="B14" s="17"/>
@@ -1817,13 +1798,10 @@
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="40"/>
-      <c r="K14" t="s">
-        <v>55</v>
-      </c>
+      <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="46">
         <v>0.125</v>
       </c>
       <c r="B15" s="20"/>
@@ -1832,10 +1810,10 @@
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="41"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46">
+      <c r="A16" s="45">
         <v>0.13541666666666699</v>
       </c>
       <c r="B16" s="17"/>
@@ -1844,10 +1822,10 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
-      <c r="H16" s="40"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
+      <c r="H16" s="39"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46">
         <v>0.14583333333333301</v>
       </c>
       <c r="B17" s="20"/>
@@ -1856,10 +1834,10 @@
       <c r="E17" s="21"/>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="41"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46">
+      <c r="H17" s="40"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45">
         <v>0.15625</v>
       </c>
       <c r="B18" s="17"/>
@@ -1868,10 +1846,10 @@
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="40"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="47">
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46">
         <v>0.16666666666666699</v>
       </c>
       <c r="B19" s="20"/>
@@ -1880,10 +1858,10 @@
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="41"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46">
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="45">
         <v>0.17708333333333301</v>
       </c>
       <c r="B20" s="17"/>
@@ -1892,11 +1870,10 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="40"/>
-      <c r="K20" s="30"/>
-    </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47">
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="46">
         <v>0.1875</v>
       </c>
       <c r="B21" s="20"/>
@@ -1905,48 +1882,48 @@
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="41"/>
-    </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46">
+      <c r="H21" s="40"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="45">
         <v>0.19791666666666699</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="42"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47">
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="41"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="46">
         <v>0.20833333333333301</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="54"/>
-    </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="45">
         <v>0.21875</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="43"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47">
+      <c r="B24" s="32"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="46">
         <v>0.22916666666666699</v>
       </c>
       <c r="B25" s="20"/>
@@ -1955,10 +1932,10 @@
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="41"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46">
+      <c r="H25" s="40"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45">
         <v>0.23958333333333301</v>
       </c>
       <c r="B26" s="17"/>
@@ -1967,10 +1944,10 @@
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="40"/>
-    </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47">
+      <c r="H26" s="39"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="46">
         <v>0.25</v>
       </c>
       <c r="B27" s="20"/>
@@ -1979,10 +1956,10 @@
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="41"/>
-    </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="46">
+      <c r="H27" s="40"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45">
         <v>0.26041666666666702</v>
       </c>
       <c r="B28" s="17"/>
@@ -1991,10 +1968,10 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47">
+      <c r="H28" s="39"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="46">
         <v>0.27083333333333298</v>
       </c>
       <c r="B29" s="20"/>
@@ -2003,10 +1980,10 @@
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="41"/>
-    </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46">
+      <c r="H29" s="40"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="45">
         <v>0.28125</v>
       </c>
       <c r="B30" s="17"/>
@@ -2015,10 +1992,10 @@
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
-      <c r="H30" s="40"/>
-    </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47">
+      <c r="H30" s="39"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="46">
         <v>0.29166666666666702</v>
       </c>
       <c r="B31" s="20"/>
@@ -2027,10 +2004,10 @@
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="41"/>
-    </row>
-    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="46">
+      <c r="H31" s="40"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="45">
         <v>0.30208333333333298</v>
       </c>
       <c r="B32" s="17"/>
@@ -2039,10 +2016,10 @@
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
-      <c r="H32" s="40"/>
+      <c r="H32" s="39"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="47">
+      <c r="A33" s="46">
         <v>0.3125</v>
       </c>
       <c r="B33" s="20"/>
@@ -2051,10 +2028,10 @@
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="41"/>
+      <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
+      <c r="A34" s="45">
         <v>0.32291666666666702</v>
       </c>
       <c r="B34" s="17"/>
@@ -2063,10 +2040,10 @@
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
-      <c r="H34" s="40"/>
+      <c r="H34" s="39"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47">
+      <c r="A35" s="46">
         <v>0.33333333333333298</v>
       </c>
       <c r="B35" s="20"/>
@@ -2075,10 +2052,10 @@
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="41"/>
+      <c r="H35" s="40"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46">
+      <c r="A36" s="45">
         <v>0.343749999999999</v>
       </c>
       <c r="B36" s="17"/>
@@ -2087,10 +2064,10 @@
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
-      <c r="H36" s="40"/>
+      <c r="H36" s="39"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="47">
+      <c r="A37" s="46">
         <v>0.35416666666666502</v>
       </c>
       <c r="B37" s="20"/>
@@ -2099,10 +2076,10 @@
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="41"/>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46">
+      <c r="A38" s="45">
         <v>0.36458333333333098</v>
       </c>
       <c r="B38" s="17"/>
@@ -2111,10 +2088,10 @@
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
-      <c r="H38" s="40"/>
+      <c r="H38" s="39"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="47">
+      <c r="A39" s="46">
         <v>0.374999999999997</v>
       </c>
       <c r="B39" s="20"/>
@@ -2123,10 +2100,10 @@
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="41"/>
+      <c r="H39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46">
+      <c r="A40" s="45">
         <v>0.38541666666666302</v>
       </c>
       <c r="B40" s="17"/>
@@ -2135,10 +2112,10 @@
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
-      <c r="H40" s="40"/>
+      <c r="H40" s="39"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47">
+      <c r="A41" s="46">
         <v>0.39583333333332898</v>
       </c>
       <c r="B41" s="20"/>
@@ -2147,10 +2124,10 @@
       <c r="E41" s="21"/>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="41"/>
+      <c r="H41" s="40"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="46">
+      <c r="A42" s="45">
         <v>0.406249999999995</v>
       </c>
       <c r="B42" s="17"/>
@@ -2159,10 +2136,10 @@
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="40"/>
+      <c r="H42" s="39"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47">
+      <c r="A43" s="46">
         <v>0.41666666666666102</v>
       </c>
       <c r="B43" s="20"/>
@@ -2171,10 +2148,10 @@
       <c r="E43" s="21"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
-      <c r="H43" s="41"/>
+      <c r="H43" s="40"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="46">
+      <c r="A44" s="45">
         <v>0.42708333333332699</v>
       </c>
       <c r="B44" s="17"/>
@@ -2183,10 +2160,10 @@
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
-      <c r="H44" s="40"/>
+      <c r="H44" s="39"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47">
+      <c r="A45" s="46">
         <v>0.43749999999999301</v>
       </c>
       <c r="B45" s="20"/>
@@ -2195,10 +2172,10 @@
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
       <c r="G45" s="21"/>
-      <c r="H45" s="41"/>
+      <c r="H45" s="40"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="46">
+      <c r="A46" s="45">
         <v>0.44791666666665902</v>
       </c>
       <c r="B46" s="17"/>
@@ -2207,10 +2184,10 @@
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
-      <c r="H46" s="40"/>
+      <c r="H46" s="39"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="47">
+      <c r="A47" s="46">
         <v>0.45833333333332499</v>
       </c>
       <c r="B47" s="20"/>
@@ -2219,10 +2196,10 @@
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="41"/>
+      <c r="H47" s="40"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="46">
+      <c r="A48" s="45">
         <v>0.46874999999999101</v>
       </c>
       <c r="B48" s="17"/>
@@ -2231,10 +2208,10 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
-      <c r="H48" s="40"/>
+      <c r="H48" s="39"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="47">
+      <c r="A49" s="46">
         <v>0.47916666666665703</v>
       </c>
       <c r="B49" s="20"/>
@@ -2243,10 +2220,10 @@
       <c r="E49" s="21"/>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
-      <c r="H49" s="41"/>
+      <c r="H49" s="40"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="46">
+      <c r="A50" s="45">
         <v>0.48958333333332299</v>
       </c>
       <c r="B50" s="17"/>
@@ -2255,10 +2232,10 @@
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
-      <c r="H50" s="40"/>
+      <c r="H50" s="39"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="47">
+      <c r="A51" s="46">
         <v>0.49999999999998901</v>
       </c>
       <c r="B51" s="20"/>
@@ -2267,10 +2244,10 @@
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
-      <c r="H51" s="41"/>
+      <c r="H51" s="40"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="46">
+      <c r="A52" s="45">
         <v>0.51041666666665497</v>
       </c>
       <c r="B52" s="17"/>
@@ -2279,10 +2256,10 @@
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
-      <c r="H52" s="40"/>
+      <c r="H52" s="39"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="47">
+      <c r="A53" s="46">
         <v>0.52083333333332105</v>
       </c>
       <c r="B53" s="20"/>
@@ -2291,10 +2268,10 @@
       <c r="E53" s="21"/>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
-      <c r="H53" s="41"/>
+      <c r="H53" s="40"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="46">
+      <c r="A54" s="45">
         <v>0.53124999999998701</v>
       </c>
       <c r="B54" s="17"/>
@@ -2303,10 +2280,10 @@
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
-      <c r="H54" s="40"/>
+      <c r="H54" s="39"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="47">
+      <c r="A55" s="46">
         <v>0.54166666666665297</v>
       </c>
       <c r="B55" s="20"/>
@@ -2315,10 +2292,10 @@
       <c r="E55" s="21"/>
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
-      <c r="H55" s="41"/>
+      <c r="H55" s="40"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="46">
+      <c r="A56" s="45">
         <v>0.55208333333331905</v>
       </c>
       <c r="B56" s="17"/>
@@ -2327,10 +2304,10 @@
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
-      <c r="H56" s="40"/>
+      <c r="H56" s="39"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="47">
+      <c r="A57" s="46">
         <v>0.56249999999998501</v>
       </c>
       <c r="B57" s="20"/>
@@ -2339,10 +2316,10 @@
       <c r="E57" s="21"/>
       <c r="F57" s="21"/>
       <c r="G57" s="21"/>
-      <c r="H57" s="41"/>
+      <c r="H57" s="40"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="46">
+      <c r="A58" s="45">
         <v>0.57291666666665098</v>
       </c>
       <c r="B58" s="17"/>
@@ -2351,10 +2328,10 @@
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
-      <c r="H58" s="40"/>
+      <c r="H58" s="39"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="47">
+      <c r="A59" s="46">
         <v>0.58333333333331705</v>
       </c>
       <c r="B59" s="20"/>
@@ -2363,10 +2340,10 @@
       <c r="E59" s="21"/>
       <c r="F59" s="21"/>
       <c r="G59" s="21"/>
-      <c r="H59" s="41"/>
+      <c r="H59" s="40"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="46">
+      <c r="A60" s="45">
         <v>0.59374999999998201</v>
       </c>
       <c r="B60" s="17"/>
@@ -2375,10 +2352,10 @@
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
-      <c r="H60" s="40"/>
+      <c r="H60" s="39"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="47">
+      <c r="A61" s="46">
         <v>0.60416666666664798</v>
       </c>
       <c r="B61" s="20"/>
@@ -2387,10 +2364,10 @@
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
-      <c r="H61" s="41"/>
+      <c r="H61" s="40"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="46">
+      <c r="A62" s="45">
         <v>0.61458333333331405</v>
       </c>
       <c r="B62" s="17"/>
@@ -2399,10 +2376,10 @@
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
-      <c r="H62" s="40"/>
+      <c r="H62" s="39"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="47">
+      <c r="A63" s="46">
         <v>0.62499999999998002</v>
       </c>
       <c r="B63" s="20"/>
@@ -2411,10 +2388,10 @@
       <c r="E63" s="21"/>
       <c r="F63" s="21"/>
       <c r="G63" s="21"/>
-      <c r="H63" s="41"/>
+      <c r="H63" s="40"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="46">
+      <c r="A64" s="45">
         <v>0.63541666666664598</v>
       </c>
       <c r="B64" s="17"/>
@@ -2423,10 +2400,10 @@
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
-      <c r="H64" s="40"/>
+      <c r="H64" s="39"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="47">
+      <c r="A65" s="46">
         <v>0.64583333333331205</v>
       </c>
       <c r="B65" s="20"/>
@@ -2435,10 +2412,10 @@
       <c r="E65" s="21"/>
       <c r="F65" s="21"/>
       <c r="G65" s="21"/>
-      <c r="H65" s="41"/>
+      <c r="H65" s="40"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="46">
+      <c r="A66" s="45">
         <v>0.65624999999997802</v>
       </c>
       <c r="B66" s="17"/>
@@ -2447,10 +2424,10 @@
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
-      <c r="H66" s="40"/>
+      <c r="H66" s="39"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="47">
+      <c r="A67" s="46">
         <v>0.66666666666664398</v>
       </c>
       <c r="B67" s="20"/>
@@ -2459,10 +2436,10 @@
       <c r="E67" s="21"/>
       <c r="F67" s="21"/>
       <c r="G67" s="21"/>
-      <c r="H67" s="41"/>
+      <c r="H67" s="40"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="46">
+      <c r="A68" s="45">
         <v>0.67708333333330994</v>
       </c>
       <c r="B68" s="17"/>
@@ -2471,10 +2448,10 @@
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
-      <c r="H68" s="40"/>
+      <c r="H68" s="39"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="47">
+      <c r="A69" s="46">
         <v>0.68749999999997602</v>
       </c>
       <c r="B69" s="20"/>
@@ -2483,10 +2460,10 @@
       <c r="E69" s="21"/>
       <c r="F69" s="21"/>
       <c r="G69" s="21"/>
-      <c r="H69" s="41"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="46">
+      <c r="A70" s="45">
         <v>0.69791666666664198</v>
       </c>
       <c r="B70" s="17"/>
@@ -2495,10 +2472,10 @@
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
-      <c r="H70" s="40"/>
+      <c r="H70" s="39"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="47">
+      <c r="A71" s="46">
         <v>0.70833333333330795</v>
       </c>
       <c r="B71" s="20"/>
@@ -2507,10 +2484,10 @@
       <c r="E71" s="21"/>
       <c r="F71" s="21"/>
       <c r="G71" s="21"/>
-      <c r="H71" s="41"/>
+      <c r="H71" s="40"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="46">
+      <c r="A72" s="45">
         <v>0.71874999999997402</v>
       </c>
       <c r="B72" s="17"/>
@@ -2519,10 +2496,10 @@
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
       <c r="G72" s="18"/>
-      <c r="H72" s="40"/>
+      <c r="H72" s="39"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="47">
+      <c r="A73" s="46">
         <v>0.72916666666663998</v>
       </c>
       <c r="B73" s="20"/>
@@ -2531,10 +2508,10 @@
       <c r="E73" s="21"/>
       <c r="F73" s="21"/>
       <c r="G73" s="21"/>
-      <c r="H73" s="41"/>
+      <c r="H73" s="40"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="46">
+      <c r="A74" s="45">
         <v>0.73958333333330595</v>
       </c>
       <c r="B74" s="17"/>
@@ -2543,10 +2520,10 @@
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
       <c r="G74" s="18"/>
-      <c r="H74" s="40"/>
+      <c r="H74" s="39"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="47">
+      <c r="A75" s="46">
         <v>0.74999999999997202</v>
       </c>
       <c r="B75" s="20"/>
@@ -2555,10 +2532,10 @@
       <c r="E75" s="21"/>
       <c r="F75" s="21"/>
       <c r="G75" s="21"/>
-      <c r="H75" s="41"/>
+      <c r="H75" s="40"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="46">
+      <c r="A76" s="45">
         <v>0.76041666666663799</v>
       </c>
       <c r="B76" s="17"/>
@@ -2567,10 +2544,10 @@
       <c r="E76" s="18"/>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
-      <c r="H76" s="40"/>
+      <c r="H76" s="39"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="47">
+      <c r="A77" s="46">
         <v>0.77083333333330395</v>
       </c>
       <c r="B77" s="20"/>
@@ -2579,10 +2556,10 @@
       <c r="E77" s="21"/>
       <c r="F77" s="21"/>
       <c r="G77" s="21"/>
-      <c r="H77" s="41"/>
+      <c r="H77" s="40"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="46">
+      <c r="A78" s="45">
         <v>0.78124999999997002</v>
       </c>
       <c r="B78" s="17"/>
@@ -2591,10 +2568,10 @@
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
-      <c r="H78" s="40"/>
+      <c r="H78" s="39"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="47">
+      <c r="A79" s="46">
         <v>0.79166666666663699</v>
       </c>
       <c r="B79" s="20"/>
@@ -2603,10 +2580,10 @@
       <c r="E79" s="21"/>
       <c r="F79" s="21"/>
       <c r="G79" s="21"/>
-      <c r="H79" s="41"/>
+      <c r="H79" s="40"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="46">
+      <c r="A80" s="45">
         <v>0.80208333333330295</v>
       </c>
       <c r="B80" s="17"/>
@@ -2615,10 +2592,10 @@
       <c r="E80" s="18"/>
       <c r="F80" s="18"/>
       <c r="G80" s="18"/>
-      <c r="H80" s="40"/>
+      <c r="H80" s="39"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="47">
+      <c r="A81" s="46">
         <v>0.81249999999996902</v>
       </c>
       <c r="B81" s="20"/>
@@ -2627,10 +2604,10 @@
       <c r="E81" s="21"/>
       <c r="F81" s="21"/>
       <c r="G81" s="21"/>
-      <c r="H81" s="41"/>
+      <c r="H81" s="40"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="46">
+      <c r="A82" s="45">
         <v>0.82291666666663499</v>
       </c>
       <c r="B82" s="17"/>
@@ -2639,10 +2616,10 @@
       <c r="E82" s="18"/>
       <c r="F82" s="18"/>
       <c r="G82" s="18"/>
-      <c r="H82" s="40"/>
+      <c r="H82" s="39"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="47">
+      <c r="A83" s="46">
         <v>0.83333333333330095</v>
       </c>
       <c r="B83" s="20"/>
@@ -2651,10 +2628,10 @@
       <c r="E83" s="21"/>
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
-      <c r="H83" s="41"/>
+      <c r="H83" s="40"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="46">
+      <c r="A84" s="45">
         <v>0.84374999999996703</v>
       </c>
       <c r="B84" s="17"/>
@@ -2663,10 +2640,10 @@
       <c r="E84" s="18"/>
       <c r="F84" s="18"/>
       <c r="G84" s="18"/>
-      <c r="H84" s="40"/>
+      <c r="H84" s="39"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="47">
+      <c r="A85" s="46">
         <v>0.85416666666663299</v>
       </c>
       <c r="B85" s="20"/>
@@ -2675,48 +2652,48 @@
       <c r="E85" s="21"/>
       <c r="F85" s="21"/>
       <c r="G85" s="21"/>
-      <c r="H85" s="41"/>
+      <c r="H85" s="40"/>
     </row>
     <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="46">
+      <c r="A86" s="45">
         <v>0.86458333333329895</v>
       </c>
-      <c r="B86" s="31"/>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="32"/>
-      <c r="H86" s="42"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="31"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
+      <c r="H86" s="41"/>
     </row>
     <row r="87" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="47">
+      <c r="A87" s="46">
         <v>0.87499999999996303</v>
       </c>
-      <c r="B87" s="52" t="s">
+      <c r="B87" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="C87" s="53"/>
-      <c r="D87" s="53"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="53"/>
-      <c r="G87" s="53"/>
-      <c r="H87" s="54"/>
+      <c r="C87" s="52"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+      <c r="H87" s="53"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="46">
+      <c r="A88" s="45">
         <v>0.88541666666662899</v>
       </c>
-      <c r="B88" s="33"/>
-      <c r="C88" s="34"/>
-      <c r="D88" s="34"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="34"/>
-      <c r="G88" s="34"/>
-      <c r="H88" s="43"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
+      <c r="H88" s="42"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="47">
+      <c r="A89" s="46">
         <v>0.89583333333329496</v>
       </c>
       <c r="B89" s="20"/>
@@ -2725,10 +2702,10 @@
       <c r="E89" s="21"/>
       <c r="F89" s="21"/>
       <c r="G89" s="21"/>
-      <c r="H89" s="41"/>
+      <c r="H89" s="40"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="46">
+      <c r="A90" s="45">
         <v>0.90624999999996103</v>
       </c>
       <c r="B90" s="17"/>
@@ -2737,10 +2714,10 @@
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
       <c r="G90" s="18"/>
-      <c r="H90" s="40"/>
+      <c r="H90" s="39"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="47">
+      <c r="A91" s="46">
         <v>0.91666666666662699</v>
       </c>
       <c r="B91" s="20"/>
@@ -2749,10 +2726,10 @@
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
       <c r="G91" s="21"/>
-      <c r="H91" s="41"/>
+      <c r="H91" s="40"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="46">
+      <c r="A92" s="45">
         <v>0.92708333333329296</v>
       </c>
       <c r="B92" s="17"/>
@@ -2761,10 +2738,10 @@
       <c r="E92" s="18"/>
       <c r="F92" s="18"/>
       <c r="G92" s="18"/>
-      <c r="H92" s="40"/>
+      <c r="H92" s="39"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="47">
+      <c r="A93" s="46">
         <v>0.93749999999995903</v>
       </c>
       <c r="B93" s="20"/>
@@ -2773,10 +2750,10 @@
       <c r="E93" s="21"/>
       <c r="F93" s="21"/>
       <c r="G93" s="21"/>
-      <c r="H93" s="41"/>
+      <c r="H93" s="40"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="46">
+      <c r="A94" s="45">
         <v>0.947916666666625</v>
       </c>
       <c r="B94" s="17"/>
@@ -2785,10 +2762,10 @@
       <c r="E94" s="18"/>
       <c r="F94" s="18"/>
       <c r="G94" s="18"/>
-      <c r="H94" s="40"/>
+      <c r="H94" s="39"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="47">
+      <c r="A95" s="46">
         <v>0.95833333333329096</v>
       </c>
       <c r="B95" s="20"/>
@@ -2797,10 +2774,10 @@
       <c r="E95" s="21"/>
       <c r="F95" s="21"/>
       <c r="G95" s="21"/>
-      <c r="H95" s="41"/>
+      <c r="H95" s="40"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="46">
+      <c r="A96" s="45">
         <v>0.96874999999995703</v>
       </c>
       <c r="B96" s="17"/>
@@ -2809,10 +2786,10 @@
       <c r="E96" s="18"/>
       <c r="F96" s="18"/>
       <c r="G96" s="18"/>
-      <c r="H96" s="40"/>
+      <c r="H96" s="39"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="47">
+      <c r="A97" s="46">
         <v>0.979166666666623</v>
       </c>
       <c r="B97" s="20"/>
@@ -2821,19 +2798,19 @@
       <c r="E97" s="21"/>
       <c r="F97" s="21"/>
       <c r="G97" s="21"/>
-      <c r="H97" s="41"/>
+      <c r="H97" s="40"/>
     </row>
     <row r="98" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="48">
+      <c r="A98" s="47">
         <v>0.98958333333328896</v>
       </c>
-      <c r="B98" s="35"/>
-      <c r="C98" s="36"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="36"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="44"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="35"/>
+      <c r="F98" s="35"/>
+      <c r="G98" s="35"/>
+      <c r="H98" s="43"/>
     </row>
     <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>